<commit_message>
feat: business knowledge memory (OpenClaw-style) + Control UI business knowledge page, remember command, GET/PUT api, cache invalidation
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/data/test_three.xlsx
+++ b/data/test_three.xlsx
@@ -441,51 +441,51 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>32管卡</t>
+          <t>PVC50止水节</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>8010071432</t>
+          <t>8020023215</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>管卡(PPR配件)印尼绿色dn32 (1")联塑</t>
+          <t>穿楼板预埋接头(止水节)PVC-U排水配件白色dn50(h118)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PVC50止水节</t>
+          <t>50直接</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>8020023215</t>
+          <t>8020020755</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>穿楼板预埋接头(止水节)PVC-U排水配件白色dn50(h118)</t>
+          <t>直通(管箍)PVC-U排水配件白色 dn50</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>PPR25管</t>
+          <t>110直接</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>8010062266</t>
+          <t>8020020757</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>(IDN)PPR冷给水直管S5(1.0MPa)印尼绿色dn25 (3/4") 4M/根联塑</t>
+          <t>直通(管箍)PVC-U排水配件白色 dn110</t>
         </is>
       </c>
     </row>

</xml_diff>